<commit_message>
track liberos + set gender limits on each team
</commit_message>
<xml_diff>
--- a/test/simple_test_data.xlsx
+++ b/test/simple_test_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jingqi/Desktop/teampartition/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jingqi/Desktop/teampartition/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60B21B0-5E01-0948-9085-0C65707187A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75751F25-B16F-EA43-9237-75C1AF4BA597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="27980" windowHeight="18380" xr2:uid="{8F58AEF8-0A0C-344B-AB88-3ED362C15D30}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="40">
   <si>
     <t>Setter</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>Conflict 7</t>
+  </si>
+  <si>
+    <t>Libero</t>
   </si>
 </sst>
 </file>
@@ -546,7 +549,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEDB53DD-9CE0-324D-9E65-939BBD020834}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -559,10 +562,10 @@
   <cols>
     <col min="1" max="1" width="16.83203125" customWidth="1"/>
     <col min="2" max="3" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="16.83203125" customWidth="1"/>
+    <col min="11" max="17" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -585,34 +588,37 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
         <v>0</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>34</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>35</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>36</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>37</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -633,29 +639,29 @@
       <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>20</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>21</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>22</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>26</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>32</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -679,11 +685,11 @@
       <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -704,8 +710,11 @@
       <c r="F4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -726,11 +735,11 @@
       <c r="F5" t="s">
         <v>12</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -754,11 +763,11 @@
       <c r="G6" t="s">
         <v>8</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -779,14 +788,14 @@
       <c r="F7" t="s">
         <v>11</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>31</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -807,17 +816,17 @@
       <c r="F8" t="s">
         <v>11</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>10</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>32</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -838,14 +847,14 @@
       <c r="F9" t="s">
         <v>7</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>32</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -866,14 +875,14 @@
       <c r="F10" t="s">
         <v>11</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>10</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -894,11 +903,11 @@
       <c r="F11" t="s">
         <v>11</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -919,11 +928,11 @@
       <c r="F12" t="s">
         <v>11</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -947,14 +956,14 @@
       <c r="G13" t="s">
         <v>7</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>10</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -975,11 +984,14 @@
       <c r="F14" t="s">
         <v>8</v>
       </c>
-      <c r="J14" t="s">
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1001,7 +1013,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1022,18 +1034,18 @@
       <c r="F16" t="s">
         <v>12</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K16">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L16">
     <sortCondition ref="D2:D16"/>
     <sortCondition ref="C2:C16"/>
     <sortCondition ref="B2:B16"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:P1048576" xr:uid="{7C74D076-EA55-1047-A177-90DE1DE45E39}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:Q1048576" xr:uid="{7C74D076-EA55-1047-A177-90DE1DE45E39}">
       <formula1>$A:$A</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>